<commit_message>
Show ms_level CV term properly
</commit_message>
<xml_diff>
--- a/examples/1_1-Metabolomics_Draft/MTBLS263.xlsx
+++ b/examples/1_1-Metabolomics_Draft/MTBLS263.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="172" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -674,13 +674,13 @@
     <t>ms_run[1]:index=274 | ms_run[1]:index=290 | ms_run[2]:index=274 | ms_run[2]:index=290 | ms_run[3]:index=270 | ms_run[3]:index=288 | ms_run[4]:index=268 | ms_run[4]:index=284 | ms_run[5]:index=266 | ms_run[5]:index=282 | ms_run[6]:index=266 | ms_run[6]:index=282</t>
   </si>
   <si>
-    <t>[MS,MS,ms level,2]</t>
+    <t>[MS,MS:100511,ms level,2]</t>
   </si>
   <si>
     <t>ms_run[1]:index=281 | ms_run[2]:index=277 | ms_run[3]:index=279 | ms_run[4]:index=273 | ms_run[5]:index=271 | ms_run[6]:index=271</t>
   </si>
   <si>
-    <t>[MS,MS,ms level,1]</t>
+    <t>[MS,MS:100511,ms level,1]</t>
   </si>
   <si>
     <t>ms_run[1]:index=301 | ms_run[2]:index=297 | ms_run[3]:index=299 | ms_run[4]:index=291 | ms_run[5]:index=289 | ms_run[6]:index=289</t>
@@ -829,16 +829,15 @@
   </sheetPr>
   <dimension ref="A1:AA113"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.46428571428571"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="26.8112244897959"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7397959183673"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4591836734694"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8010204081633"/>
@@ -850,7 +849,7 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.219387755102"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="332.683673469388"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.1020408163265"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.0714285714286"/>
     <col collapsed="false" hidden="false" max="20" min="18" style="0" width="22.6887755102041"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.2397959183673"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="22.1275510204082"/>

</xml_diff>